<commit_message>
Jan 14 Bug Fixes
</commit_message>
<xml_diff>
--- a/SM2.xlsx
+++ b/SM2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HarrySherman\OneDrive - August Group\Personal OneDrive\Coding\Copilot Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://augustgroupcom-my.sharepoint.com/personal/harry_augustgroup_com/Documents/Documents/GitHub/MasterProcessor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F3C4C4B-3A02-4369-B0F5-EF3C007540C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{0F3C4C4B-3A02-4369-B0F5-EF3C007540C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A54AB82-78D2-4439-BC39-8810DB1C398B}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="10944" windowHeight="7968" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dec 08" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Security ID</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>CAD</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -591,7 +594,7 @@
         <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
         <v>19</v>
@@ -683,6 +686,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C1F0D067A12012479498FC325B78D79D" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ecebec2cf55b5bbaf456311009ff3829">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d092c0fb-b5b9-48b9-8171-6ecd1e40e399" xmlns:ns3="31d2e8a2-6be5-431b-8140-e1f547e63473" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cd07b31856fb8cfd63f72d87dab673e5" ns2:_="" ns3:_="">
     <xsd:import namespace="d092c0fb-b5b9-48b9-8171-6ecd1e40e399"/>
@@ -937,16 +949,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{190B3BD7-3B70-45E1-9731-4A1454026C9B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{585AD502-2FE9-4F4D-B070-C81B527E78E5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -963,12 +974,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{190B3BD7-3B70-45E1-9731-4A1454026C9B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>